<commit_message>
Change discount to 4%
</commit_message>
<xml_diff>
--- a/suppxls/Scen_ShellImprovement-setup.xlsx
+++ b/suppxls/Scen_ShellImprovement-setup.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5E1302-1DFE-4D8B-9E97-8002AD3F12B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8B8925-E786-4C9F-9C7C-EE907DB62C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1695" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1695" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="17" r:id="rId1"/>
     <sheet name="basedem_drsh" sheetId="18" r:id="rId2"/>
     <sheet name="basedem_drot" sheetId="19" r:id="rId3"/>
-    <sheet name="veda" sheetId="16" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F16434-42CB-4657-81C1-D4CE1BD7CEFC}">
   <dimension ref="B3:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8636,7 +8636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E903F0BA-7879-4E52-9B65-D85A41EDE771}">
   <dimension ref="B4:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>